<commit_message>
adding primer barcode IDs to primerBarcodeList
</commit_message>
<xml_diff>
--- a/data/indexed_primers/Kozich_DualIndex_V4_primers.xlsx
+++ b/data/indexed_primers/Kozich_DualIndex_V4_primers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="-26880" yWindow="3560" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="107">
   <si>
     <t>plate</t>
   </si>
@@ -244,6 +244,102 @@
   </si>
   <si>
     <t>CAAGCAGAAGACGGCATACGAGAT</t>
+  </si>
+  <si>
+    <t>515F</t>
+  </si>
+  <si>
+    <t>806R</t>
+  </si>
+  <si>
+    <t>SA501</t>
+  </si>
+  <si>
+    <t>SA502</t>
+  </si>
+  <si>
+    <t>SA503</t>
+  </si>
+  <si>
+    <t>SA504</t>
+  </si>
+  <si>
+    <t>SA505</t>
+  </si>
+  <si>
+    <t>SA506</t>
+  </si>
+  <si>
+    <t>SA507</t>
+  </si>
+  <si>
+    <t>SA508</t>
+  </si>
+  <si>
+    <t>SB501</t>
+  </si>
+  <si>
+    <t>SB502</t>
+  </si>
+  <si>
+    <t>SB503</t>
+  </si>
+  <si>
+    <t>SB504</t>
+  </si>
+  <si>
+    <t>SB505</t>
+  </si>
+  <si>
+    <t>SB506</t>
+  </si>
+  <si>
+    <t>SB507</t>
+  </si>
+  <si>
+    <t>SB508</t>
+  </si>
+  <si>
+    <t>SA701</t>
+  </si>
+  <si>
+    <t>SA702</t>
+  </si>
+  <si>
+    <t>SA703</t>
+  </si>
+  <si>
+    <t>SA704</t>
+  </si>
+  <si>
+    <t>SA705</t>
+  </si>
+  <si>
+    <t>SA706</t>
+  </si>
+  <si>
+    <t>SA707</t>
+  </si>
+  <si>
+    <t>SA708</t>
+  </si>
+  <si>
+    <t>SA709</t>
+  </si>
+  <si>
+    <t>SA710</t>
+  </si>
+  <si>
+    <t>SA711</t>
+  </si>
+  <si>
+    <t>SA712</t>
+  </si>
+  <si>
+    <t>location_16S_ID</t>
+  </si>
+  <si>
+    <t>ref_paper_ID</t>
   </si>
 </sst>
 </file>
@@ -315,8 +411,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -339,17 +443,25 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -679,24 +791,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="33.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="1"/>
-    <col min="8" max="8" width="22.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="76" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="22.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="76" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,34 +821,40 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-      <c r="O1" s="3"/>
+      <c r="O1" s="2"/>
       <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="Q1" s="3"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -745,31 +865,37 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="S2" s="4"/>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="M2" s="3"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="U2" s="4"/>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -780,30 +906,36 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="N3" s="4"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="M3" s="3"/>
+      <c r="P3" s="4"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="U3" s="4"/>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -814,30 +946,36 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="N4" s="4"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="S4" s="4"/>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="M4" s="3"/>
+      <c r="P4" s="4"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="U4" s="4"/>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -848,30 +986,36 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="N5" s="4"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="S5" s="4"/>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="M5" s="3"/>
+      <c r="P5" s="4"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="U5" s="4"/>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -882,30 +1026,36 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="N6" s="4"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="S6" s="4"/>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="M6" s="3"/>
+      <c r="P6" s="4"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="U6" s="4"/>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -916,30 +1066,36 @@
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="3"/>
-      <c r="N7" s="4"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="S7" s="4"/>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="M7" s="3"/>
+      <c r="P7" s="4"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="U7" s="4"/>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -950,30 +1106,36 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="N8" s="4"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="S8" s="4"/>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="M8" s="3"/>
+      <c r="P8" s="4"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="U8" s="4"/>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -984,30 +1146,36 @@
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K9" s="3"/>
-      <c r="N9" s="4"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="S9" s="4"/>
-    </row>
-    <row r="10" spans="1:19">
+      <c r="M9" s="3"/>
+      <c r="P9" s="4"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="U9" s="4"/>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1018,25 +1186,31 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:21">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1047,25 +1221,31 @@
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="H11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:21">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1076,25 +1256,31 @@
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:21">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1105,25 +1291,31 @@
         <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="H13" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:21">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1134,25 +1326,31 @@
         <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="H14" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="J14" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:21">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1163,25 +1361,31 @@
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="G15" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="H15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:21">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1192,25 +1396,31 @@
         <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="G16" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="H16" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:21">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1221,25 +1431,31 @@
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:21">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -1250,25 +1466,31 @@
         <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="J18" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:21">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -1279,25 +1501,31 @@
         <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="G19" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="H19" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="J19" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:21">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -1308,25 +1536,31 @@
         <v>11</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="H20" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:21">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1337,25 +1571,31 @@
         <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="G21" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="H21" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:21">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -1366,31 +1606,37 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="3"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="S22" s="4"/>
-    </row>
-    <row r="23" spans="1:19">
+      <c r="M22" s="3"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="U22" s="4"/>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -1401,30 +1647,36 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K23" s="3"/>
-      <c r="N23" s="4"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="S23" s="4"/>
-    </row>
-    <row r="24" spans="1:19">
+      <c r="M23" s="3"/>
+      <c r="P23" s="4"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="U23" s="4"/>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -1435,30 +1687,36 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K24" s="3"/>
-      <c r="N24" s="4"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="S24" s="4"/>
-    </row>
-    <row r="25" spans="1:19">
+      <c r="M24" s="3"/>
+      <c r="P24" s="4"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="U24" s="4"/>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" s="1">
         <v>2</v>
       </c>
@@ -1469,30 +1727,36 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="3"/>
-      <c r="N25" s="4"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="S25" s="4"/>
-    </row>
-    <row r="26" spans="1:19">
+      <c r="M25" s="3"/>
+      <c r="P25" s="4"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="U25" s="4"/>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -1503,30 +1767,36 @@
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K26" s="3"/>
-      <c r="N26" s="4"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="S26" s="4"/>
-    </row>
-    <row r="27" spans="1:19">
+      <c r="M26" s="3"/>
+      <c r="P26" s="4"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="U26" s="4"/>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" s="1">
         <v>2</v>
       </c>
@@ -1537,30 +1807,36 @@
         <v>6</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K27" s="3"/>
-      <c r="N27" s="4"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="S27" s="4"/>
-    </row>
-    <row r="28" spans="1:19">
+      <c r="M27" s="3"/>
+      <c r="P27" s="4"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="U27" s="4"/>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" s="1">
         <v>2</v>
       </c>
@@ -1571,30 +1847,36 @@
         <v>7</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K28" s="3"/>
-      <c r="N28" s="4"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="S28" s="4"/>
-    </row>
-    <row r="29" spans="1:19">
+      <c r="M28" s="3"/>
+      <c r="P28" s="4"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="U28" s="4"/>
+    </row>
+    <row r="29" spans="1:21">
       <c r="A29" s="1">
         <v>2</v>
       </c>
@@ -1605,30 +1887,36 @@
         <v>8</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K29" s="3"/>
-      <c r="N29" s="4"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="S29" s="4"/>
-    </row>
-    <row r="30" spans="1:19">
+      <c r="M29" s="3"/>
+      <c r="P29" s="4"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="U29" s="4"/>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" s="1">
         <v>2</v>
       </c>
@@ -1639,25 +1927,31 @@
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="G30" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="H30" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="J30" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:21">
       <c r="A31" s="1">
         <v>2</v>
       </c>
@@ -1668,25 +1962,31 @@
         <v>2</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="G31" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="H31" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="J31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:21">
       <c r="A32" s="1">
         <v>2</v>
       </c>
@@ -1697,25 +1997,31 @@
         <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="H32" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="J32" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:11">
       <c r="A33" s="1">
         <v>2</v>
       </c>
@@ -1726,25 +2032,31 @@
         <v>4</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="G33" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="H33" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="J33" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:11">
       <c r="A34" s="1">
         <v>2</v>
       </c>
@@ -1755,25 +2067,31 @@
         <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="H34" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="J34" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:11">
       <c r="A35" s="1">
         <v>2</v>
       </c>
@@ -1784,25 +2102,31 @@
         <v>6</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="G35" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="H35" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="J35" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:11">
       <c r="A36" s="1">
         <v>2</v>
       </c>
@@ -1813,25 +2137,31 @@
         <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="G36" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="H36" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="J36" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:11">
       <c r="A37" s="1">
         <v>2</v>
       </c>
@@ -1842,25 +2172,31 @@
         <v>8</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="G37" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="H37" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="J37" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:11">
       <c r="A38" s="1">
         <v>2</v>
       </c>
@@ -1871,25 +2207,31 @@
         <v>9</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="G38" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="H38" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="J38" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:11">
       <c r="A39" s="1">
         <v>2</v>
       </c>
@@ -1900,25 +2242,31 @@
         <v>10</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="G39" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="H39" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="J39" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:11">
       <c r="A40" s="1">
         <v>2</v>
       </c>
@@ -1929,25 +2277,31 @@
         <v>11</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="H40" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="J40" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:11">
       <c r="A41" s="1">
         <v>2</v>
       </c>
@@ -1958,21 +2312,27 @@
         <v>12</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="G41" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="H41" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H41" s="5" t="s">
+      <c r="J41" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>